<commit_message>
Added the Office scene.
</commit_message>
<xml_diff>
--- a/article/graphics_thesis.xlsx
+++ b/article/graphics_thesis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="893" firstSheet="5" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="893" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Algorithm Overview" sheetId="1" r:id="rId1"/>
@@ -29120,8 +29120,8 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="B1:AV41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T26" sqref="T26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AA40" sqref="AA40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31053,7 +31053,7 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="B1:AY68"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>